<commit_message>
[what] fix implementation - Paillier encryption and decryption - update sample data - add more logs for execution - add md file for explainations
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -32,11 +32,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="4">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>

</xml_diff>